<commit_message>
add comments to bulk parser, bug fixes
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/bulk_entry.xlsx
+++ b/bio_diversity/static/data_templates/bulk_entry.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,137 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Stoyel, Quentin</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name of the site</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Description of Site</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>River Code, eg. BSR, SMA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional. Tributary Name, must match code in database</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Optional. Subriver name, must match code in database. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional.
+Eg 45.0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional.
+Eg. 45.1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional.
+Eg. -65.0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional.
+Eg. -64.9</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
@@ -60,13 +191,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -386,11 +523,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,6 +567,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -437,7 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -464,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add comment row to all templates, fix movement unit tests
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/bulk_entry.xlsx
+++ b/bio_diversity/static/data_templates/bulk_entry.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoyelq\Desktop\Work\dm_apps\dm_apps\bio_diversity\static\data_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED0D8F2-575A-4785-B146-CE6A12C2CE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="2430" yWindow="1335" windowWidth="23535" windowHeight="13620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="1" r:id="rId1"/>
@@ -26,139 +27,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Stoyel, Quentin</author>
-  </authors>
-  <commentList>
-    <comment ref="A3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Name of the site</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Description of Site</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>River Code, eg. BSR, SMA</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional. Tributary Name, must match code in database</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Optional. Subriver name, must match code in database. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional.
-Eg 45.0</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional.
-Eg. 45.1</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional.
-Eg. -65.0</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional.
-Eg. -64.9</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -185,12 +55,45 @@
   </si>
   <si>
     <t>Max Long</t>
+  </si>
+  <si>
+    <t>Name of the site</t>
+  </si>
+  <si>
+    <t>Description of site</t>
+  </si>
+  <si>
+    <t>River Code. Eg. SMA, BSR</t>
+  </si>
+  <si>
+    <t>Optional, Name must match code in database.</t>
+  </si>
+  <si>
+    <t>Optional, Subriver name must match code in database</t>
+  </si>
+  <si>
+    <t>Optional. Eg. 45.0</t>
+  </si>
+  <si>
+    <t>Optional. Eg. 45.1</t>
+  </si>
+  <si>
+    <t>Optional. Eg. -65.1</t>
+  </si>
+  <si>
+    <t>Optional. Eg. -65.0</t>
+  </si>
+  <si>
+    <t>Name of the container</t>
+  </si>
+  <si>
+    <t>Description of container</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -200,8 +103,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -220,7 +123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -237,13 +140,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,84 +460,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B3"/>
@@ -609,14 +470,102 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -625,9 +574,45 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B3"/>
@@ -635,15 +620,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add docs to nav bar, add tankdets into bulk entry
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/bulk_entry.xlsx
+++ b/bio_diversity/static/data_templates/bulk_entry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoyelq\Desktop\Work\dm_apps\dm_apps\bio_diversity\static\data_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED0D8F2-575A-4785-B146-CE6A12C2CE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E037BE06-2DDF-4B31-B77F-35921C9D884A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2430" yWindow="1335" windowWidth="23535" windowHeight="13620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Description of container</t>
+  </si>
+  <si>
+    <t>Effective Surface Area</t>
+  </si>
+  <si>
+    <t>Effective surface area of the tank that can be used to calculate water volume</t>
   </si>
 </sst>
 </file>
@@ -540,7 +546,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:B3"/>
+  <dimension ref="A2:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -550,22 +556,29 @@
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>